<commit_message>
Made the code cleaner for APIConnect and process_to_JSON.py
</commit_message>
<xml_diff>
--- a/backend/output.xlsx
+++ b/backend/output.xlsx
@@ -14,22 +14,982 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>Error</t>
-  </si>
-  <si>
-    <t>message</t>
-  </si>
-  <si>
-    <t>There is an error when searching from AI. code: 'Reference'</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="70">
+  <si>
+    <t>Land Use Document Type</t>
+  </si>
+  <si>
+    <t>File name</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>AI Title</t>
+  </si>
+  <si>
+    <t>Section #</t>
+  </si>
+  <si>
+    <t>Section Title</t>
+  </si>
+  <si>
+    <t>Search Terms</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Page Number</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>Proposed amendment</t>
+  </si>
+  <si>
+    <t>Rationale</t>
+  </si>
+  <si>
+    <t>Zoning and Development By-law</t>
+  </si>
+  <si>
+    <t>zoning-by-law-section-2.pdf</t>
+  </si>
+  <si>
+    <t>zoning-by-law-section-4.pdf</t>
+  </si>
+  <si>
+    <t>zoning-by-law-section-5.pdf</t>
+  </si>
+  <si>
+    <t>2 - Definitions</t>
+  </si>
+  <si>
+    <t>4 - Development Permits</t>
+  </si>
+  <si>
+    <t>5 - By-law Relaxations and Powers of Discretion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">City of Vancouver April 2024
+Zoning and Development By-law 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">City of Vancouver October 2023
+Zoning and Development By-law 
+</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>44.1.6</t>
+  </si>
+  <si>
+    <t>4.8</t>
+  </si>
+  <si>
+    <t>4.8.1</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Term Definition</t>
+  </si>
+  <si>
+    <t>Exemptions from Development Permit Requirements</t>
+  </si>
+  <si>
+    <t>Required Setbacks and Balcony Projections</t>
+  </si>
+  <si>
+    <t>parking</t>
+  </si>
+  <si>
+    <t>https://bylaws.vancouver.ca/zoning/zoning-by-law-section-2.pdf#page=28</t>
+  </si>
+  <si>
+    <t>https://bylaws.vancouver.ca/zoning/zoning-by-law-section-2.pdf#page=35</t>
+  </si>
+  <si>
+    <t>https://bylaws.vancouver.ca/zoning/zoning-by-law-section-2.pdf#page=44</t>
+  </si>
+  <si>
+    <t>https://bylaws.vancouver.ca/zoning/zoning-by-law-section-4.pdf#page=2</t>
+  </si>
+  <si>
+    <t>https://bylaws.vancouver.ca/zoning/zoning-by-law-section-4.pdf#page=7</t>
+  </si>
+  <si>
+    <t>https://bylaws.vancouver.ca/zoning/zoning-by-law-section-4.pdf#page=8</t>
+  </si>
+  <si>
+    <t>https://bylaws.vancouver.ca/zoning/zoning-by-law-section-4.pdf#page=9</t>
+  </si>
+  <si>
+    <t>https://bylaws.vancouver.ca/zoning/zoning-by-law-section-5.pdf#page=3</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>City of Vancouver April 2024Zoning and Development By-law Page 28Section 2Term DefinitionPPackaging Plant The use of premises for the boxing, crating or related packaging of goods or material brought specifically to the premises for that purpose. TPaper Manufacturing The use of premises for the manufacturing of paper. MPaper Products ManufacturingThe use of premises for the manufacturing of paper products, but does not include Paper Manufacturing, Pulp Manufacturing, Petroleum Products or Coal Products Manufacturing, or Printing or Publishing. MParking Area An open area of land other than a street or lane, used or intended to be used to provide space for the parking or storage of motor vehicles, and includes parking spaces, loading spaces, manoeuvring aisles and other areas providing access to parking or loading spaces, but does not include an area providing 4 or fewer spaces accessory to a residential use and may include the retail sale of electricity for the purpose of charging motor vehicles. PParking Garage A structure or a portion of a structure which is principally used or intended to be used for the parking or storage of motor vehicles, but does not include a structure providing 4 or fewer spaces accessory to a residential use and may include the retail sale of electricity for the purpose of charging motor vehicles. PParking Uses Any or all of the following land uses:Parking Area ; Parking Garage . PPartial Storey  The uppermost level of a building where the floor area, existing, proposed or as may be extended over open-to-below space, and having a minimum ceiling height of 1. 2 m, is limited to a specified proportion of the storey immediately below</t>
+  </si>
+  <si>
+    <t>TPaper Manufacturing The use of premises for the manufacturing of paper. MPaper Products ManufacturingThe use of premises for the manufacturing of paper products, but does not include Paper Manufacturing, Pulp Manufacturing, Petroleum Products or Coal Products Manufacturing, or Printing or Publishing. MParking Area An open area of land other than a street or lane, used or intended to be used to provide space for the parking or storage of motor vehicles, and includes parking spaces, loading spaces, manoeuvring aisles and other areas providing access to parking or loading spaces, but does not include an area providing 4 or fewer spaces accessory to a residential use and may include the retail sale of electricity for the purpose of charging motor vehicles. PParking Garage A structure or a portion of a structure which is principally used or intended to be used for the parking or storage of motor vehicles, but does not include a structure providing 4 or fewer spaces accessory to a residential use and may include the retail sale of electricity for the purpose of charging motor vehicles. PParking Uses Any or all of the following land uses:Parking Area ; Parking Garage . PPartial Storey  The uppermost level of a building where the floor area, existing, proposed or as may be extended over open-to-below space, and having a minimum ceiling height of 1. 2 m, is limited to a specified proportion of the storey immediately below. Passive House Building CertifierA person internationally accredited by the Passive House Institute in Darmstadt, Germany for the purpose of certifying buildings as being designed in accordance with its Passive House standards</t>
+  </si>
+  <si>
+    <t>MPaper Products ManufacturingThe use of premises for the manufacturing of paper products, but does not include Paper Manufacturing, Pulp Manufacturing, Petroleum Products or Coal Products Manufacturing, or Printing or Publishing. MParking Area An open area of land other than a street or lane, used or intended to be used to provide space for the parking or storage of motor vehicles, and includes parking spaces, loading spaces, manoeuvring aisles and other areas providing access to parking or loading spaces, but does not include an area providing 4 or fewer spaces accessory to a residential use and may include the retail sale of electricity for the purpose of charging motor vehicles. PParking Garage A structure or a portion of a structure which is principally used or intended to be used for the parking or storage of motor vehicles, but does not include a structure providing 4 or fewer spaces accessory to a residential use and may include the retail sale of electricity for the purpose of charging motor vehicles. PParking Uses Any or all of the following land uses:Parking Area ; Parking Garage . PPartial Storey  The uppermost level of a building where the floor area, existing, proposed or as may be extended over open-to-below space, and having a minimum ceiling height of 1. 2 m, is limited to a specified proportion of the storey immediately below. Passive House Building CertifierA person internationally accredited by the Passive House Institute in Darmstadt, Germany for the purpose of certifying buildings as being designed in accordance with its Passive House standards. Partial StoreyPartial Storey≥1</t>
+  </si>
+  <si>
+    <t>City of Vancouver April 2024Zoning and Development By-law Page 35Section 2Term DefinitionRestaurant - Class 2 The use of premises for the primary purpose of selling and serving prepared food to the public during all hours of operation, where the premises include at least 17 indoor or outdoor seats for customers consuming food purchased on the premises, and where live entertainment, including the use of non-amplified or amplified musical instruments and disc jockey mixing turntables and patron participation such as karaoke, dancing and open microphone performing, may be available. SRestaurant - Drive-In The use of premises for the sale of prepared food to the public where parking is provided and customers are encouraged to eat in their motor vehicles on the site, but does not include drive-through service. SRetail To offer to sell or rent, or to sell or rent, merchandise to a consumer who buys or rents the merchandise as the ultimate consumer or end user, being the last person in the chain of distribution, for personal consumption or use and not for further sale or rent. Retail Store The use of premises to retail merchandise, including merchandise manufactured on the premises, if the total floor area used for manufacturing does not exceed 300 m2, but which does not include any other retail uses listed in this Section 2  or included in a lumber and building materials establishment. RRetail Uses Any or all of the following land uses:Adult Retail Store ; Cannabis Store ; Farmers’ Market ;Furniture or Appliance Store ; Gasoline Station - Full Serve ; Gasoline Station - Split Island ; Grocery or Drug Store ;Grocery Store with Liquor Store ; Liquor Store ;Neighbourhood Grocery Store ; R</t>
+  </si>
+  <si>
+    <t>City of Vancouver April 2024Zoning and Development By-law Page 44Section 2Term DefinitionTransportation and Storage UsesAny or all of the following land uses:Aircraft Landing Place ; Booming Ground ;Bulk Data Storage ; Cold Storage Plant ; Grain Elevator ;Marine Terminal or Berth ; Mini-Storage Warehouse ; Packaging Plant ;Railway Station or Rail Yard ; Stockyard ;Storage Warehouse ; Storage Yard ;Taxicab or Limousine Station ; Truck Terminal or Courier Depot ; Weighing or Inspection Station ; Works Yard . TTransportation Equipment ManufacturingThe use of premises for the manufacturing of aircraft, railroad rolling stock, ships, boats, truck or bus bodies, truck trailers, snowmobiles or motor vehicles. MTriplex A building containing 3 principal dwelling  units, but does not include a Multiple Conversion Dwelling. DTruck Terminal or Courier DepotThe use of premises for the parking and servicing of trailers, containers, trucks, and other motor vehicles involved in commercial transport, cartage, moving, delivery, or related goods movement. TUUltimate Property Line The property line that results when an anticipated or partially dedicated lane or street abuts a site, and that becomes the property boundary for the purposes of measuring required yards. Urban Farm - Class A The use of land, with or without a principal building, for the cultivation of fruits or vegetables for sale. A</t>
+  </si>
+  <si>
+    <t>City of Vancouver April 2024Zoning and Development By-law Page 2Section 44. 1. 6 No development permit may be issued until plans or drawings have been submitted that show that the proposed development or change of use is in compliance with the provisions of any by-law regulating the provision of parking and loading within the City. 4. 2 Development Permit Application Time Limits4. 2. 1 Unless otherwise approved, refused or subject to limitations in time as may be imposed by the Director of Planning or Development Permit Board, any development permit application will be void 12 months from the date of application</t>
+  </si>
+  <si>
+    <t>4. 8 Exemptions from Development Permit Requirements4. 8. 1 A person who complies in all other respects with this by-law, the Parking By-law , other City by-laws, any official development plan, and any development permit, to the extent any of them apply to that person’ s site, need not obtain a development permit for the following development and uses:(a) the maintenance or minor repair of any building, structure or use, other than a building, structure, use or site designated under the Heritage By-law or located in an HA  district, except that the Director of Planning may exempt an applicant from the requirement to obtain a development permit in an HA District where the Director of Planning is satisfied that the maintenance or minor repair does not contravene this by-law  or any applicable official development plan, or Council approved policies or guidelines;(b) the construction or use of an accessory building or an accessory use that is permitted as an outright approval use in the applicable district schedule and is located on the same site as the principal building or use;(c) the construction or placing of tool sheds, construction shacks, scaffolding or similar temporary buildings required for a limited period of time, intended solely to serve a development or activity that is being carried out in compliance with this by-law , and is located on the same site or on an adjoining parcel;(d) the installation, inspection, repair or renewal of sewers, mains, pipes, cables, wires or other similar apparatus required in connection with any lawful use of buildings or land;(e) the construction and maintenance of that part of a public utility placed in or upon a public thoroughfare or public utility easement;(f) the construction, widening, improvement, maintenance or repair of any highway, lane, street, bridge or other public thoroughfare;(g) the demolition of any building, except for a building:(i) used for residential rental accommodation,(ii) listed on the Vancouver Heritage Register, or(iii) used for residential accommodation in the R1-1 or First Shaughnessy districts,</t>
+  </si>
+  <si>
+    <t>8. 1(g)  does not apply to any building that is residential rental accommodation subject to the provisions of section 10. 14. 3 , subject to a demolition order, subject to demolition as a condition of subdivision approval, or used for residential accommodation in the R1-1 or First Shaughnessy districts, not listed on the Vancouver Heritage Register, and for which a building permit has been issued to demolish by deconstruction;(h) the placing or maintenance of any fence or similar enclosure structure except those requiring the permission of the Director of Planning or Development Permit Board;(i)  the keeping of not more than 2 boarders or lodgers or the keeping of not more than 5 foster or 8 daycare  children in each dwelling  unit;(j)  the keeping of animals or birds for domestic purposes, except as otherwise prohibited or regulated by the Animal Control By-law;(k) the renting of no more than 1 off-street parking space accessory to a single detached house or a duplex, provided that the space is surplus to the minimum parking requirements of the dwelling ;(l)  the provision of recreation rooms or extra bedrooms in the basement of a single detached house or duplex;(m) the engaging in a homecraft;(n) the change in use from a lawfully existing use listed in Column A to a use listed opposite in Column B:Column A: From Column B: To(i) Multiple conversion dwelling  or rooming house. Single detached house. (ii) Multiple conversion dwelling .  Multiple conversion dwelling  containing the same or fewer units in total, except in the RT-4, RT-4A, RT-4AN, RT-4N, RT-5, RT-5N, RT-6 , RT-7 , RT-8, RT-9, RT-10, RT-10N, RT-11 , RT-11N , RM-1, RM-1N, RM-7, RM-7N, RM-7AN , RM-8, RM-8A, RM-8N, RM-8AN, RM-9 , RM-9A, RM-9N, RM-9AN, RM-9BN, RM-10 , RM-10N, RM-11, RM-11N, RM-12N or First Shaughnessy districts. (iii) Except as provided in section 4</t>
+  </si>
+  <si>
+    <t>City of Vancouver April 2024Zoning and Development By-law Page 9Section 4Column A: From Column B: To(iv) Any use located in an industrial district and listed in the applicable district schedule as an outright or conditional approval use, but not including a storage warehouse or any use where the number of parking and loading spaces has been relaxed. Any outright use listed in the same district schedule. (v) 1 or more of the following outright or conditional approval uses in a district: general office, retail store, health care office, barber shop or beauty salon, and beauty and wellness centre;Any of the other outright or conditional approval uses in a district listed in column A, provided the total floor space does not exceed 300m². (o) the construction of antennae, including satellite dishes, provided:(i) they are located in the rear yard and are no higher than 1.  9 m above the existing grade, or in the case of satellite dishes, comply with the height regulations of the district in which they are located and do not exceed 77 cm in diameter, and(ii) if they are located in an R district, they are used for domestic purposes;(p) the installation of a mural on a hoarding where at least 50% of the hoarding is located on a street or lane;(q) the repair or alteration of any building, structure or use to rectify an unsafe condition if correction of such unsafe condition has been ordered by the City Building Inspector;(r) outside the projected area of the outermost walls of all principal or accessory buildings on the site, the installation, repair, or replacement of impermeable materials permitted in any of the R1 district schedules;(s) the installation and maintenance of a public bike share station as part of public bike share, provided that the public bike share station:(i) does not include any enclosed structures,(ii) is automated,(iii) does not interfere with any public works, facilities or amenities, and(iv) is part of a network comprised of no fewer than 50 public bike share stations;(t) the installation and maintenance of a shared e-scooter station as part of a shared e-scooter system, provided that the shared e-scooter station:(i) does not include any enclosed structures,(ii) is automated,</t>
+  </si>
+  <si>
+    <t>City of Vancouver October 2023Zoning and Development By-law Page 3Section 5(h) required setbacks to off-street parking areas where, in the opinion of the Director of Planning, the landscaping provided or to be provided is adequate to warrant such decrease, except that in the C-1 district  or an R district, no decrease may be granted that has the effect of decreasing the front yard to less than the required depth of an adjoining front yard; and(i)  the maximum projection of balconies into required yards, horizontal daylight control angle s, and limitations on building depth. 5. 2. 2 Despite anything to the contrary in this by-law, if(a) the construction or alteration of, or addition to, a building is to include enhanced accessibility to and from the building by way of ramps, lifts, or other like means for persons facing barriers to access because they have a loss or reduction of functional ability or activity; and(b) the Director of Planning considers all applicable Council guidelines and policies,then the Director of Planning may vary the requirements in the applicable district schedule regarding yards, setbacks, site coverage, impermeability, building depth, and side door entrance to the extent necessary to allow such enhanced accessibility. 5</t>
+  </si>
+  <si>
+    <t>Strike out  and includes parking spaces, loading spaces, manoeuvring aisles and other areas providing access to parking or loading spaces, but does not include an area providing 4 or fewer spaces accessory to a residential use and substitute 'See parking by-law'</t>
+  </si>
+  <si>
+    <t>No Change</t>
+  </si>
+  <si>
+    <t>Remove mentions of specific parking space requirements and replace with 'see parking by-law'</t>
+  </si>
+  <si>
+    <r>
+      <t>City of Vancouver April 2024Zoning and Development By-law Page 28Section 2Term DefinitionPPackaging Plant The use of premises for the boxing, crating or related packaging of goods or material brought specifically to the premises for that purpose. TPaper Manufacturing The use of premises for the manufacturing of paper. MPaper Products ManufacturingThe use of premises for the manufacturing of paper products, but does not include Paper Manufacturing, Pulp Manufacturing, Petroleum Products or Coal Products Manufacturing, or Printing or Publishing. M</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Parking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Area An open area of land other than a street or lane, used or intended to be used to provide space for the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>parking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or storage of motor vehicles, and includes </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>parking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> spaces, loading spaces, manoeuvring aisles and other areas providing access to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>parking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or loading spaces, but does not include an area providing 4 or fewer spaces accessory to a residential use and may include the retail sale of electricity for the purpose of charging motor vehicles. P</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Parking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Garage A structure or a portion of a structure which is principally used or intended to be used for the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>parking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or storage of motor vehicles, but does not include a structure providing 4 or fewer spaces accessory to a residential use and may include the retail sale of electricity for the purpose of charging motor vehicles. P</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Parking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Uses Any or all of the following land uses:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Parking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Area ; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Parking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Garage . PPartial Storey  The uppermost level of a building where the floor area, existing, proposed or as may be extended over open-to-below space, and having a minimum ceiling height of 1. 2 m, is limited to a specified proportion of the storey immediately below</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>TPaper Manufacturing The use of premises for the manufacturing of paper. MPaper Products ManufacturingThe use of premises for the manufacturing of paper products, but does not include Paper Manufacturing, Pulp Manufacturing, Petroleum Products or Coal Products Manufacturing, or Printing or Publishing. M</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Parking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Area An open area of land other than a street or lane, used or intended to be used to provide space for the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>parking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or storage of motor vehicles, and includes </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>parking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> spaces, loading spaces, manoeuvring aisles and other areas providing access to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>parking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or loading spaces, but does not include an area providing 4 or fewer spaces accessory to a residential use and may include the retail sale of electricity for the purpose of charging motor vehicles. P</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Parking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Garage A structure or a portion of a structure which is principally used or intended to be used for the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>parking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or storage of motor vehicles, but does not include a structure providing 4 or fewer spaces accessory to a residential use and may include the retail sale of electricity for the purpose of charging motor vehicles. P</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Parking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Uses Any or all of the following land uses:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Parking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Area ; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Parking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Garage . PPartial Storey  The uppermost level of a building where the floor area, existing, proposed or as may be extended over open-to-below space, and having a minimum ceiling height of 1. 2 m, is limited to a specified proportion of the storey immediately below. Passive House Building CertifierA person internationally accredited by the Passive House Institute in Darmstadt, Germany for the purpose of certifying buildings as being designed in accordance with its Passive House standards</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>MPaper Products ManufacturingThe use of premises for the manufacturing of paper products, but does not include Paper Manufacturing, Pulp Manufacturing, Petroleum Products or Coal Products Manufacturing, or Printing or Publishing. M</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Parking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Area An open area of land other than a street or lane, used or intended to be used to provide space for the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>parking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or storage of motor vehicles, and includes </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>parking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> spaces, loading spaces, manoeuvring aisles and other areas providing access to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>parking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or loading spaces, but does not include an area providing 4 or fewer spaces accessory to a residential use and may include the retail sale of electricity for the purpose of charging motor vehicles. P</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Parking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Garage A structure or a portion of a structure which is principally used or intended to be used for the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>parking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or storage of motor vehicles, but does not include a structure providing 4 or fewer spaces accessory to a residential use and may include the retail sale of electricity for the purpose of charging motor vehicles. P</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Parking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Uses Any or all of the following land uses:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Parking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Area ; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Parking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Garage . PPartial Storey  The uppermost level of a building where the floor area, existing, proposed or as may be extended over open-to-below space, and having a minimum ceiling height of 1. 2 m, is limited to a specified proportion of the storey immediately below. Passive House Building CertifierA person internationally accredited by the Passive House Institute in Darmstadt, Germany for the purpose of certifying buildings as being designed in accordance with its Passive House standards. Partial StoreyPartial Storey≥1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">City of Vancouver April 2024Zoning and Development By-law Page 35Section 2Term DefinitionRestaurant - Class 2 The use of premises for the primary purpose of selling and serving prepared food to the public during all hours of operation, where the premises include at least 17 indoor or outdoor seats for customers consuming food purchased on the premises, and where live entertainment, including the use of non-amplified or amplified musical instruments and disc jockey mixing turntables and patron participation such as karaoke, dancing and open microphone performing, may be available. SRestaurant - Drive-In The use of premises for the sale of prepared food to the public where </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>parking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is provided and customers are encouraged to eat in their motor vehicles on the site, but does not include drive-through service. SRetail To offer to sell or rent, or to sell or rent, merchandise to a consumer who buys or rents the merchandise as the ultimate consumer or end user, being the last person in the chain of distribution, for personal consumption or use and not for further sale or rent. Retail Store The use of premises to retail merchandise, including merchandise manufactured on the premises, if the total floor area used for manufacturing does not exceed 300 m2, but which does not include any other retail uses listed in this Section 2  or included in a lumber and building materials establishment. RRetail Uses Any or all of the following land uses:Adult Retail Store ; Cannabis Store ; Farmers’ Market ;Furniture or Appliance Store ; Gasoline Station - Full Serve ; Gasoline Station - Split Island ; Grocery or Drug Store ;Grocery Store with Liquor Store ; Liquor Store ;Neighbourhood Grocery Store ; R</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">City of Vancouver April 2024Zoning and Development By-law Page 44Section 2Term DefinitionTransportation and Storage UsesAny or all of the following land uses:Aircraft Landing Place ; Booming Ground ;Bulk Data Storage ; Cold Storage Plant ; Grain Elevator ;Marine Terminal or Berth ; Mini-Storage Warehouse ; Packaging Plant ;Railway Station or Rail Yard ; Stockyard ;Storage Warehouse ; Storage Yard ;Taxicab or Limousine Station ; Truck Terminal or Courier Depot ; Weighing or Inspection Station ; Works Yard . TTransportation Equipment ManufacturingThe use of premises for the manufacturing of aircraft, railroad rolling stock, ships, boats, truck or bus bodies, truck trailers, snowmobiles or motor vehicles. MTriplex A building containing 3 principal dwelling  units, but does not include a Multiple Conversion Dwelling. DTruck Terminal or Courier DepotThe use of premises for the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>parking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and servicing of trailers, containers, trucks, and other motor vehicles involved in commercial transport, cartage, moving, delivery, or related goods movement. TUUltimate Property Line The property line that results when an anticipated or partially dedicated lane or street abuts a site, and that becomes the property boundary for the purposes of measuring required yards. Urban Farm - Class A The use of land, with or without a principal building, for the cultivation of fruits or vegetables for sale. A</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">City of Vancouver April 2024Zoning and Development By-law Page 2Section 44. 1. 6 No development permit may be issued until plans or drawings have been submitted that show that the proposed development or change of use is in compliance with the provisions of any by-law regulating the provision of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>parking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and loading within the City. 4. 2 Development Permit Application Time Limits4. 2. 1 Unless otherwise approved, refused or subject to limitations in time as may be imposed by the Director of Planning or Development Permit Board, any development permit application will be void 12 months from the date of application</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4. 8 Exemptions from Development Permit Requirements4. 8. 1 A person who complies in all other respects with this by-law, the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Parking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> By-law , other City by-laws, any official development plan, and any development permit, to the extent any of them apply to that person’ s site, need not obtain a development permit for the following development and uses:(a) the maintenance or minor repair of any building, structure or use, other than a building, structure, use or site designated under the Heritage By-law or located in an HA  district, except that the Director of Planning may exempt an applicant from the requirement to obtain a development permit in an HA District where the Director of Planning is satisfied that the maintenance or minor repair does not contravene this by-law  or any applicable official development plan, or Council approved policies or guidelines;(b) the construction or use of an accessory building or an accessory use that is permitted as an outright approval use in the applicable district schedule and is located on the same site as the principal building or use;(c) the construction or placing of tool sheds, construction shacks, scaffolding or similar temporary buildings required for a limited period of time, intended solely to serve a development or activity that is being carried out in compliance with this by-law , and is located on the same site or on an adjoining parcel;(d) the installation, inspection, repair or renewal of sewers, mains, pipes, cables, wires or other similar apparatus required in connection with any lawful use of buildings or land;(e) the construction and maintenance of that part of a public utility placed in or upon a public thoroughfare or public utility easement;(f) the construction, widening, improvement, maintenance or repair of any highway, lane, street, bridge or other public thoroughfare;(g) the demolition of any building, except for a building:(i) used for residential rental accommodation,(ii) listed on the Vancouver Heritage Register, or(iii) used for residential accommodation in the R1-1 or First Shaughnessy districts,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">8. 1(g)  does not apply to any building that is residential rental accommodation subject to the provisions of section 10. 14. 3 , subject to a demolition order, subject to demolition as a condition of subdivision approval, or used for residential accommodation in the R1-1 or First Shaughnessy districts, not listed on the Vancouver Heritage Register, and for which a building permit has been issued to demolish by deconstruction;(h) the placing or maintenance of any fence or similar enclosure structure except those requiring the permission of the Director of Planning or Development Permit Board;(i)  the keeping of not more than 2 boarders or lodgers or the keeping of not more than 5 foster or 8 daycare  children in each dwelling  unit;(j)  the keeping of animals or birds for domestic purposes, except as otherwise prohibited or regulated by the Animal Control By-law;(k) the renting of no more than 1 off-street </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>parking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> space accessory to a single detached house or a duplex, provided that the space is surplus to the minimum </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>parking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> requirements of the dwelling ;(l)  the provision of recreation rooms or extra bedrooms in the basement of a single detached house or duplex;(m) the engaging in a homecraft;(n) the change in use from a lawfully existing use listed in Column A to a use listed opposite in Column B:Column A: From Column B: To(i) Multiple conversion dwelling  or rooming house. Single detached house. (ii) Multiple conversion dwelling .  Multiple conversion dwelling  containing the same or fewer units in total, except in the RT-4, RT-4A, RT-4AN, RT-4N, RT-5, RT-5N, RT-6 , RT-7 , RT-8, RT-9, RT-10, RT-10N, RT-11 , RT-11N , RM-1, RM-1N, RM-7, RM-7N, RM-7AN , RM-8, RM-8A, RM-8N, RM-8AN, RM-9 , RM-9A, RM-9N, RM-9AN, RM-9BN, RM-10 , RM-10N, RM-11, RM-11N, RM-12N or First Shaughnessy districts. (iii) Except as provided in section 4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">City of Vancouver April 2024Zoning and Development By-law Page 9Section 4Column A: From Column B: To(iv) Any use located in an industrial district and listed in the applicable district schedule as an outright or conditional approval use, but not including a storage warehouse or any use where the number of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>parking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and loading spaces has been relaxed. Any outright use listed in the same district schedule. (v) 1 or more of the following outright or conditional approval uses in a district: general office, retail store, health care office, barber shop or beauty salon, and beauty and wellness centre;Any of the other outright or conditional approval uses in a district listed in column A, provided the total floor space does not exceed 300m². (o) the construction of antennae, including satellite dishes, provided:(i) they are located in the rear yard and are no higher than 1.  9 m above the existing grade, or in the case of satellite dishes, comply with the height regulations of the district in which they are located and do not exceed 77 cm in diameter, and(ii) if they are located in an R district, they are used for domestic purposes;(p) the installation of a mural on a hoarding where at least 50% of the hoarding is located on a street or lane;(q) the repair or alteration of any building, structure or use to rectify an unsafe condition if correction of such unsafe condition has been ordered by the City Building Inspector;(r) outside the projected area of the outermost walls of all principal or accessory buildings on the site, the installation, repair, or replacement of impermeable materials permitted in any of the R1 district schedules;(s) the installation and maintenance of a public bike share station as part of public bike share, provided that the public bike share station:(i) does not include any enclosed structures,(ii) is automated,(iii) does not interfere with any public works, facilities or amenities, and(iv) is part of a network comprised of no fewer than 50 public bike share stations;(t) the installation and maintenance of a shared e-scooter station as part of a shared e-scooter system, provided that the shared e-scooter station:(i) does not include any enclosed structures,(ii) is automated,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">City of Vancouver October 2023Zoning and Development By-law Page 3Section 5(h) required setbacks to off-street </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>parking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> areas where, in the opinion of the Director of Planning, the landscaping provided or to be provided is adequate to warrant such decrease, except that in the C-1 district  or an R district, no decrease may be granted that has the effect of decreasing the front yard to less than the required depth of an adjoining front yard; and(i)  the maximum projection of balconies into required yards, horizontal daylight control angle s, and limitations on building depth. 5. 2. 2 Despite anything to the contrary in this by-law, if(a) the construction or alteration of, or addition to, a building is to include enhanced accessibility to and from the building by way of ramps, lifts, or other like means for persons facing barriers to access because they have a loss or reduction of functional ability or activity; and(b) the Director of Planning considers all applicable Council guidelines and policies,then the Director of Planning may vary the requirements in the applicable district schedule regarding yards, setbacks, site coverage, impermeability, building depth, and side door entrance to the extent necessary to allow such enhanced accessibility. 5</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -44,6 +1004,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -78,16 +1045,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -380,26 +1353,443 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:12">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K2" t="s">
+        <v>57</v>
+      </c>
+      <c r="L2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" t="s">
+        <v>61</v>
+      </c>
+      <c r="K3" t="s">
+        <v>57</v>
+      </c>
+      <c r="L3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K4" t="s">
+        <v>57</v>
+      </c>
+      <c r="L4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J5" t="s">
+        <v>63</v>
+      </c>
+      <c r="K5" t="s">
+        <v>58</v>
+      </c>
+      <c r="L5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" t="s">
+        <v>64</v>
+      </c>
+      <c r="K6" t="s">
+        <v>58</v>
+      </c>
+      <c r="L6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" t="s">
+        <v>65</v>
+      </c>
+      <c r="K7" t="s">
+        <v>58</v>
+      </c>
+      <c r="L7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" t="s">
+        <v>43</v>
+      </c>
+      <c r="J8" t="s">
+        <v>66</v>
+      </c>
+      <c r="K8" t="s">
+        <v>58</v>
+      </c>
+      <c r="L8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I9" t="s">
+        <v>44</v>
+      </c>
+      <c r="J9" t="s">
+        <v>67</v>
+      </c>
+      <c r="K9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I10" t="s">
+        <v>45</v>
+      </c>
+      <c r="J10" t="s">
+        <v>68</v>
+      </c>
+      <c r="K10" t="s">
+        <v>58</v>
+      </c>
+      <c r="L10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11" t="s">
+        <v>46</v>
+      </c>
+      <c r="J11" t="s">
+        <v>69</v>
+      </c>
+      <c r="K11" t="s">
+        <v>58</v>
+      </c>
+      <c r="L11" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" location="page=28"/>
+    <hyperlink ref="H3" r:id="rId2" location="page=28"/>
+    <hyperlink ref="H4" r:id="rId3" location="page=28"/>
+    <hyperlink ref="H5" r:id="rId4" location="page=35"/>
+    <hyperlink ref="H6" r:id="rId5" location="page=44"/>
+    <hyperlink ref="H7" r:id="rId6" location="page=2"/>
+    <hyperlink ref="H8" r:id="rId7" location="page=7"/>
+    <hyperlink ref="H9" r:id="rId8" location="page=8"/>
+    <hyperlink ref="H10" r:id="rId9" location="page=9"/>
+    <hyperlink ref="H11" r:id="rId10" location="page=3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>